<commit_message>
#62631 Test Protocol renamed and Review sheet update with “reviewer” column
</commit_message>
<xml_diff>
--- a/Documents/External/ReviewRecords/Review_Sheet_Test_Protocol_CommLib.xlsx
+++ b/Documents/External/ReviewRecords/Review_Sheet_Test_Protocol_CommLib.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28209"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="28502"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310250098/iCloud Drive (Archive)/Documents/Platform_Releases/Platform_Release_2.2.0/Test_Protocols/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/phnl310250098/git/android-commlib-workspace/Source/commlib/Documents/External/ReviewRecords/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="70">
   <si>
     <t>Purpose</t>
   </si>
@@ -245,7 +245,19 @@
     <t>"Start discovery" is not mentioned since Android app does not suport this step yet.</t>
   </si>
   <si>
-    <t>N</t>
+    <t>Reviewer</t>
+  </si>
+  <si>
+    <t>Gerard Arts</t>
+  </si>
+  <si>
+    <t>Bas Flaton</t>
+  </si>
+  <si>
+    <t>Luis Rosa</t>
+  </si>
+  <si>
+    <t>Peter Fortuin</t>
   </si>
 </sst>
 </file>
@@ -1398,845 +1410,880 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="110" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" view="pageLayout" zoomScale="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="9.1640625" style="4"/>
-    <col min="3" max="3" width="45.5" style="4" customWidth="1"/>
-    <col min="4" max="5" width="9.1640625" style="4"/>
-    <col min="6" max="6" width="37" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="9.1640625" style="4"/>
+    <col min="1" max="1" width="11.6640625" style="4" customWidth="1"/>
+    <col min="2" max="3" width="9.1640625" style="4"/>
+    <col min="4" max="4" width="45.5" style="4" customWidth="1"/>
+    <col min="5" max="6" width="9.1640625" style="4"/>
+    <col min="7" max="7" width="37" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" s="5" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+      <c r="B1" s="15" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+    <row r="3" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-      <c r="D3" s="20"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="19"/>
       <c r="E3" s="20"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="21"/>
-    </row>
-    <row r="4" spans="1:9" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A4" s="22" t="s">
+      <c r="F3" s="20"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="21"/>
+    </row>
+    <row r="4" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="C4" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="D4" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="E4" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="25" t="s">
+      <c r="F4" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="G4" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="H4" s="25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="27"/>
+    <row r="5" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="29"/>
-      <c r="I5" s="31"/>
-    </row>
-    <row r="6" spans="1:9" customFormat="1" ht="130" x14ac:dyDescent="0.2">
-      <c r="A6" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="B6" s="27"/>
-      <c r="C6" s="32"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="34"/>
-      <c r="G6" s="35"/>
-    </row>
-    <row r="7" spans="1:9" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A7" s="27" t="s">
+      <c r="D5" s="27"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="29"/>
+      <c r="G5" s="30"/>
+      <c r="H5" s="29"/>
+      <c r="J5" s="31"/>
+    </row>
+    <row r="6" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>36</v>
       </c>
+      <c r="C6" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" s="34" t="s">
+        <v>57</v>
+      </c>
+      <c r="H6" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
       <c r="B7" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7" s="27"/>
+      <c r="D7" s="32" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="34" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="27">
+        <v>5</v>
+      </c>
+      <c r="C8" s="27"/>
+      <c r="D8" s="32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>34</v>
       </c>
-      <c r="E7" s="33" t="s">
+      <c r="F8" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="34" t="s">
-        <v>57</v>
-      </c>
-      <c r="G7" s="35" t="s">
+      <c r="G8" s="34" t="s">
+        <v>59</v>
+      </c>
+      <c r="H8" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:9" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A8" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="28" t="s">
+    <row r="9" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="27">
+        <v>7</v>
+      </c>
+      <c r="C9" s="27">
+        <v>16790</v>
+      </c>
+      <c r="D9" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>69</v>
+      </c>
+      <c r="B10" s="27">
+        <v>15</v>
+      </c>
+      <c r="C10" s="27">
+        <v>40416</v>
+      </c>
+      <c r="D10" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H10" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>67</v>
+      </c>
+      <c r="B11" s="27">
+        <v>20</v>
+      </c>
+      <c r="C11" s="27">
+        <v>18511</v>
+      </c>
+      <c r="D11" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="27">
+        <v>23</v>
+      </c>
+      <c r="C12" s="27">
+        <v>31700</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="H12" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="27"/>
+      <c r="C13" s="27">
+        <v>54008</v>
+      </c>
+      <c r="D13" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F13" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>68</v>
+      </c>
+      <c r="B14" s="27"/>
+      <c r="C14" s="27">
+        <v>58371</v>
+      </c>
+      <c r="D14" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" customFormat="1" ht="39" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="27"/>
+      <c r="C15" s="27">
+        <v>59923</v>
+      </c>
+      <c r="D15" s="32" t="s">
+        <v>50</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="34" t="s">
+        <v>51</v>
+      </c>
+      <c r="H15" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="27"/>
+      <c r="C16" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="D16" s="32" t="s">
+        <v>53</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G16" s="34" t="s">
+        <v>60</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" customFormat="1" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>68</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27">
+        <v>40236</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="F17" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G17" s="34" t="s">
+        <v>62</v>
+      </c>
+      <c r="H17" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" customFormat="1" ht="52" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" s="27"/>
+      <c r="C18" s="27">
+        <v>47904</v>
+      </c>
+      <c r="D18" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="E18" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="G18" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="H18" s="35" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>68</v>
+      </c>
+      <c r="B19" s="27"/>
+      <c r="C19" s="27">
+        <v>49881</v>
+      </c>
+      <c r="D19" s="32" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="28" t="s">
         <v>38</v>
       </c>
-      <c r="E8" s="33" t="s">
+      <c r="F19" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="F8" s="34" t="s">
-        <v>58</v>
-      </c>
-      <c r="G8" s="35" t="s">
+      <c r="G19" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H19" s="35" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="27">
-        <v>5</v>
-      </c>
-      <c r="B9" s="27"/>
-      <c r="C9" s="32" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E9" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>59</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="27">
-        <v>7</v>
-      </c>
-      <c r="B10" s="27">
-        <v>16790</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="27">
-        <v>15</v>
-      </c>
-      <c r="B11" s="27">
-        <v>40416</v>
-      </c>
-      <c r="C11" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F11" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G11" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="27">
-        <v>20</v>
-      </c>
-      <c r="B12" s="27">
-        <v>18511</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="D12" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E12" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F12" s="34" t="s">
-        <v>46</v>
-      </c>
-      <c r="G12" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="27">
-        <v>23</v>
-      </c>
-      <c r="B13" s="27">
-        <v>31700</v>
-      </c>
-      <c r="C13" s="36" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F13" s="34" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" customFormat="1" ht="39" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27">
-        <v>54008</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E14" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="F14" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G14" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27">
-        <v>58371</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E15" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F15" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" customFormat="1" ht="39" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27">
-        <v>59923</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E16" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F16" s="34" t="s">
-        <v>51</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E17" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F17" s="34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" customFormat="1" ht="26" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27">
-        <v>40236</v>
-      </c>
-      <c r="C18" s="36" t="s">
-        <v>54</v>
-      </c>
-      <c r="D18" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="E18" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F18" s="34" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" customFormat="1" ht="52" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27">
-        <v>47904</v>
-      </c>
-      <c r="C19" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="D19" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="E19" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F19" s="34" t="s">
-        <v>61</v>
-      </c>
-      <c r="G19" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27">
-        <v>49881</v>
-      </c>
-      <c r="C20" s="32" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="E20" s="33" t="s">
-        <v>43</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="35" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
+    <row r="20" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B20" s="27"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
+    </row>
+    <row r="21" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B21" s="27"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="28"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="34"/>
-      <c r="G21" s="35"/>
-    </row>
-    <row r="22" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
+      <c r="C21" s="27"/>
+      <c r="D21" s="38"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="35"/>
+    </row>
+    <row r="22" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B22" s="27"/>
-      <c r="C22" s="38"/>
-      <c r="D22" s="28"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="34"/>
-      <c r="G22" s="35"/>
-    </row>
-    <row r="23" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="32"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="33"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="35"/>
+    </row>
+    <row r="23" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B23" s="27"/>
-      <c r="C23" s="32"/>
-      <c r="D23" s="28"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="34"/>
-      <c r="G23" s="35"/>
-    </row>
-    <row r="24" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="32"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="33"/>
+      <c r="G23" s="34"/>
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B24" s="27"/>
-      <c r="C24" s="32"/>
-      <c r="D24" s="28"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="34"/>
-      <c r="G24" s="35"/>
-    </row>
-    <row r="25" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B25" s="27"/>
-      <c r="C25" s="32"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="34"/>
-      <c r="G25" s="35"/>
-    </row>
-    <row r="26" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
+      <c r="C25" s="27"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="33"/>
+      <c r="G25" s="34"/>
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B26" s="27"/>
-      <c r="C26" s="32"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="34"/>
-      <c r="G26" s="35"/>
-    </row>
-    <row r="27" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
+      <c r="C26" s="27"/>
+      <c r="D26" s="32"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="34"/>
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B27" s="27"/>
-      <c r="C27" s="32"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="34"/>
-      <c r="G27" s="35"/>
-    </row>
-    <row r="28" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
-      <c r="B28" s="27"/>
-      <c r="C28" s="32"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="35"/>
-    </row>
-    <row r="29" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="39"/>
+      <c r="C27" s="27"/>
+      <c r="D27" s="32"/>
+      <c r="E27" s="28"/>
+      <c r="F27" s="33"/>
+      <c r="G27" s="34"/>
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B28" s="39"/>
+      <c r="C28" s="27"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="28"/>
+      <c r="F28" s="33"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="35"/>
+    </row>
+    <row r="29" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B29" s="27"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="28"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="34"/>
-      <c r="G29" s="35"/>
-    </row>
-    <row r="30" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="32"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="33"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="35"/>
+    </row>
+    <row r="30" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B30" s="27"/>
-      <c r="C30" s="32"/>
-      <c r="D30" s="28"/>
-      <c r="E30" s="33"/>
-      <c r="F30" s="34"/>
-      <c r="G30" s="35"/>
-    </row>
-    <row r="31" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
+      <c r="C30" s="27"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="33"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="35"/>
+    </row>
+    <row r="31" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B31" s="27"/>
-      <c r="C31" s="32"/>
-      <c r="D31" s="28"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="34"/>
-      <c r="G31" s="35"/>
-    </row>
-    <row r="32" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
-      <c r="B32" s="40"/>
-      <c r="C32" s="38"/>
-      <c r="D32" s="28"/>
-      <c r="E32" s="33"/>
-      <c r="F32" s="34"/>
-      <c r="G32" s="35"/>
-    </row>
-    <row r="33" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="27"/>
+      <c r="C31" s="40"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="28"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="35"/>
+    </row>
+    <row r="32" spans="1:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B32" s="27"/>
+      <c r="C32" s="27"/>
+      <c r="D32" s="32"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="33"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="35"/>
+    </row>
+    <row r="33" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B33" s="27"/>
-      <c r="C33" s="32"/>
-      <c r="D33" s="28"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="35"/>
-    </row>
-    <row r="34" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="27"/>
-      <c r="B34" s="27"/>
-      <c r="C34" s="37"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="34"/>
-      <c r="G34" s="35"/>
-    </row>
-    <row r="35" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="39"/>
+      <c r="C33" s="27"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
+      <c r="H33" s="35"/>
+    </row>
+    <row r="34" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B34" s="39"/>
+      <c r="C34" s="27"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="28"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="35"/>
+    </row>
+    <row r="35" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B35" s="27"/>
-      <c r="C35" s="32"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="33"/>
-      <c r="F35" s="34"/>
-      <c r="G35" s="35"/>
-    </row>
-    <row r="36" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A36" s="27"/>
+      <c r="C35" s="27"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="28"/>
+      <c r="F35" s="33"/>
+      <c r="G35" s="34"/>
+      <c r="H35" s="35"/>
+    </row>
+    <row r="36" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B36" s="27"/>
-      <c r="C36" s="32"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="33"/>
-      <c r="F36" s="34"/>
-      <c r="G36" s="35"/>
-    </row>
-    <row r="37" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A37" s="27"/>
+      <c r="C36" s="27"/>
+      <c r="D36" s="32"/>
+      <c r="E36" s="28"/>
+      <c r="F36" s="33"/>
+      <c r="G36" s="34"/>
+      <c r="H36" s="35"/>
+    </row>
+    <row r="37" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B37" s="27"/>
-      <c r="C37" s="32"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="34"/>
-      <c r="G37" s="35"/>
-    </row>
-    <row r="38" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A38" s="27"/>
-      <c r="B38" s="27"/>
-      <c r="C38" s="32"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="33"/>
-      <c r="F38" s="34"/>
-      <c r="G38" s="35"/>
-    </row>
-    <row r="39" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A39" s="39"/>
-      <c r="B39" s="27"/>
-      <c r="C39" s="32"/>
-      <c r="D39" s="28"/>
-      <c r="E39" s="33"/>
-      <c r="F39" s="34"/>
-      <c r="G39" s="35"/>
-    </row>
-    <row r="40" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="39"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="28"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="34"/>
+      <c r="H37" s="35"/>
+    </row>
+    <row r="38" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B38" s="39"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="32"/>
+      <c r="E38" s="28"/>
+      <c r="F38" s="33"/>
+      <c r="G38" s="34"/>
+      <c r="H38" s="35"/>
+    </row>
+    <row r="39" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B39" s="39"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="32"/>
+      <c r="E39" s="28"/>
+      <c r="F39" s="33"/>
+      <c r="G39" s="34"/>
+      <c r="H39" s="35"/>
+    </row>
+    <row r="40" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B40" s="27"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="28"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="35"/>
-    </row>
-    <row r="41" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A41" s="27"/>
+      <c r="C40" s="27"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="28"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="34"/>
+      <c r="H40" s="35"/>
+    </row>
+    <row r="41" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
       <c r="B41" s="27"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="28"/>
-      <c r="E41" s="33"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="35"/>
-    </row>
-    <row r="42" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="27"/>
-      <c r="B42" s="27"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="33"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="35"/>
-    </row>
-    <row r="43" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A43" s="42"/>
-      <c r="B43" s="27"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="28"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="43"/>
-      <c r="G43" s="35"/>
-    </row>
-    <row r="44" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="42"/>
-      <c r="B44" s="27"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="28"/>
-      <c r="E44" s="35"/>
-      <c r="F44" s="43"/>
-      <c r="G44" s="35"/>
-    </row>
-    <row r="45" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A45" s="42"/>
-      <c r="B45" s="27"/>
-      <c r="C45" s="32"/>
-      <c r="D45" s="28"/>
-      <c r="E45" s="35"/>
-      <c r="F45" s="43"/>
-      <c r="G45" s="35"/>
-    </row>
-    <row r="46" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A46" s="42"/>
-      <c r="B46" s="27"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="28"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="43"/>
-      <c r="G46" s="35"/>
-    </row>
-    <row r="47" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A47" s="42"/>
-      <c r="B47" s="27"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="28"/>
-      <c r="E47" s="35"/>
-      <c r="F47" s="43"/>
-      <c r="G47" s="35"/>
-    </row>
-    <row r="48" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="42"/>
-      <c r="B48" s="27"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="28"/>
-      <c r="E48" s="35"/>
-      <c r="F48" s="43"/>
-      <c r="G48" s="35"/>
-    </row>
-    <row r="49" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="42"/>
-      <c r="B49" s="27"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="28"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="43"/>
-      <c r="G49" s="35"/>
-    </row>
-    <row r="50" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="42"/>
-      <c r="B50" s="27"/>
-      <c r="C50" s="32"/>
-      <c r="D50" s="28"/>
-      <c r="E50" s="35"/>
-      <c r="F50" s="43"/>
-      <c r="G50" s="35"/>
-    </row>
-    <row r="51" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A51" s="42"/>
-      <c r="B51" s="27"/>
-      <c r="C51" s="32"/>
-      <c r="D51" s="28"/>
-      <c r="E51" s="35"/>
-      <c r="F51" s="43"/>
-      <c r="G51" s="35"/>
-    </row>
-    <row r="52" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="42"/>
-      <c r="B52" s="27"/>
-      <c r="C52" s="32"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="43"/>
-      <c r="G52" s="35"/>
-    </row>
-    <row r="53" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="42"/>
-      <c r="B53" s="27"/>
-      <c r="C53" s="32"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="35"/>
-      <c r="F53" s="43"/>
-      <c r="G53" s="35"/>
-    </row>
-    <row r="54" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="42"/>
-      <c r="B54" s="27"/>
-      <c r="C54" s="32"/>
-      <c r="D54" s="28"/>
-      <c r="E54" s="35"/>
-      <c r="F54" s="43"/>
-      <c r="G54" s="35"/>
-    </row>
-    <row r="55" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="42"/>
-      <c r="B55" s="27"/>
-      <c r="C55" s="32"/>
-      <c r="D55" s="28"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="43"/>
-      <c r="G55" s="35"/>
-    </row>
-    <row r="56" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="42"/>
-      <c r="B56" s="27"/>
-      <c r="C56" s="32"/>
-      <c r="D56" s="28"/>
-      <c r="E56" s="35"/>
-      <c r="F56" s="43"/>
-      <c r="G56" s="35"/>
-    </row>
-    <row r="57" spans="1:7" customFormat="1" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="42"/>
-      <c r="B57" s="27"/>
-      <c r="C57" s="32"/>
-      <c r="D57" s="28"/>
-      <c r="E57" s="35"/>
-      <c r="F57" s="43"/>
-      <c r="G57" s="35"/>
+      <c r="C41" s="27"/>
+      <c r="D41" s="32"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="33"/>
+      <c r="G41" s="34"/>
+      <c r="H41" s="35"/>
+    </row>
+    <row r="42" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B42" s="42"/>
+      <c r="C42" s="27"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="28"/>
+      <c r="F42" s="35"/>
+      <c r="G42" s="43"/>
+      <c r="H42" s="35"/>
+    </row>
+    <row r="43" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B43" s="42"/>
+      <c r="C43" s="27"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="28"/>
+      <c r="F43" s="35"/>
+      <c r="G43" s="43"/>
+      <c r="H43" s="35"/>
+    </row>
+    <row r="44" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B44" s="42"/>
+      <c r="C44" s="27"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="28"/>
+      <c r="F44" s="35"/>
+      <c r="G44" s="43"/>
+      <c r="H44" s="35"/>
+    </row>
+    <row r="45" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B45" s="42"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="32"/>
+      <c r="E45" s="28"/>
+      <c r="F45" s="35"/>
+      <c r="G45" s="43"/>
+      <c r="H45" s="35"/>
+    </row>
+    <row r="46" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B46" s="42"/>
+      <c r="C46" s="27"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="28"/>
+      <c r="F46" s="35"/>
+      <c r="G46" s="43"/>
+      <c r="H46" s="35"/>
+    </row>
+    <row r="47" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B47" s="42"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="32"/>
+      <c r="E47" s="28"/>
+      <c r="F47" s="35"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="35"/>
+    </row>
+    <row r="48" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B48" s="42"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="32"/>
+      <c r="E48" s="28"/>
+      <c r="F48" s="35"/>
+      <c r="G48" s="43"/>
+      <c r="H48" s="35"/>
+    </row>
+    <row r="49" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B49" s="42"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="28"/>
+      <c r="F49" s="35"/>
+      <c r="G49" s="43"/>
+      <c r="H49" s="35"/>
+    </row>
+    <row r="50" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B50" s="42"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="32"/>
+      <c r="E50" s="28"/>
+      <c r="F50" s="35"/>
+      <c r="G50" s="43"/>
+      <c r="H50" s="35"/>
+    </row>
+    <row r="51" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B51" s="42"/>
+      <c r="C51" s="27"/>
+      <c r="D51" s="32"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="35"/>
+      <c r="G51" s="43"/>
+      <c r="H51" s="35"/>
+    </row>
+    <row r="52" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B52" s="42"/>
+      <c r="C52" s="27"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="28"/>
+      <c r="F52" s="35"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="35"/>
+    </row>
+    <row r="53" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B53" s="42"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="32"/>
+      <c r="E53" s="28"/>
+      <c r="F53" s="35"/>
+      <c r="G53" s="43"/>
+      <c r="H53" s="35"/>
+    </row>
+    <row r="54" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B54" s="42"/>
+      <c r="C54" s="27"/>
+      <c r="D54" s="32"/>
+      <c r="E54" s="28"/>
+      <c r="F54" s="35"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="35"/>
+    </row>
+    <row r="55" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B55" s="42"/>
+      <c r="C55" s="27"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="28"/>
+      <c r="F55" s="35"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="35"/>
+    </row>
+    <row r="56" spans="2:8" customFormat="1" ht="15" x14ac:dyDescent="0.2">
+      <c r="B56" s="42"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="28"/>
+      <c r="F56" s="35"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="35"/>
     </row>
   </sheetData>
   <phoneticPr fontId="13" type="noConversion"/>
-  <conditionalFormatting sqref="D5:D9 D11:D12">
+  <conditionalFormatting sqref="E10:E11 E5:E8">
     <cfRule type="expression" dxfId="29" priority="37" stopIfTrue="1">
-      <formula>OR(D5="S",D5="Ma",D5="mi",D5="cl",D5="Q")</formula>
+      <formula>OR(E5="S",E5="Ma",E5="mi",E5="cl",E5="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="28" priority="38" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D42:D57">
+  <conditionalFormatting sqref="E41:E56">
     <cfRule type="expression" dxfId="27" priority="31" stopIfTrue="1">
-      <formula>OR(D42="S",D42="Ma",D42="mi",D42="cl",D42="Q")</formula>
+      <formula>OR(E41="S",E41="Ma",E41="mi",E41="cl",E41="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="26" priority="32" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D24">
+  <conditionalFormatting sqref="E23">
     <cfRule type="expression" dxfId="25" priority="27" stopIfTrue="1">
-      <formula>OR(D24="S",D24="Ma",D24="mi",D24="cl",D24="Q")</formula>
+      <formula>OR(E23="S",E23="Ma",E23="mi",E23="cl",E23="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="24" priority="28" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D41">
+  <conditionalFormatting sqref="E40">
     <cfRule type="expression" dxfId="23" priority="25" stopIfTrue="1">
-      <formula>OR(D41="S",D41="Ma",D41="mi",D41="cl",D41="Q")</formula>
+      <formula>OR(E40="S",E40="Ma",E40="mi",E40="cl",E40="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="22" priority="26" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D23">
+  <conditionalFormatting sqref="E21:E22">
     <cfRule type="expression" dxfId="21" priority="23" stopIfTrue="1">
-      <formula>OR(D22="S",D22="Ma",D22="mi",D22="cl",D22="Q")</formula>
+      <formula>OR(E21="S",E21="Ma",E21="mi",E21="cl",E21="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="20" priority="24" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D21">
+  <conditionalFormatting sqref="E20">
     <cfRule type="expression" dxfId="19" priority="21" stopIfTrue="1">
-      <formula>OR(D21="S",D21="Ma",D21="mi",D21="cl",D21="Q")</formula>
+      <formula>OR(E20="S",E20="Ma",E20="mi",E20="cl",E20="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="18" priority="22" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D33 D25 D27:D31">
+  <conditionalFormatting sqref="E32 E24 E26:E30">
     <cfRule type="expression" dxfId="17" priority="19" stopIfTrue="1">
-      <formula>OR(D25="S",D25="Ma",D25="mi",D25="cl",D25="Q")</formula>
+      <formula>OR(E24="S",E24="Ma",E24="mi",E24="cl",E24="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="16" priority="20" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D34">
+  <conditionalFormatting sqref="E33">
     <cfRule type="expression" dxfId="15" priority="17" stopIfTrue="1">
-      <formula>OR(D34="S",D34="Ma",D34="mi",D34="cl",D34="Q")</formula>
+      <formula>OR(E33="S",E33="Ma",E33="mi",E33="cl",E33="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="14" priority="18" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D32">
+  <conditionalFormatting sqref="E31">
     <cfRule type="expression" dxfId="13" priority="15" stopIfTrue="1">
-      <formula>OR(D32="S",D32="Ma",D32="mi",D32="cl",D32="Q")</formula>
+      <formula>OR(E31="S",E31="Ma",E31="mi",E31="cl",E31="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="16" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D35 D37:D40">
+  <conditionalFormatting sqref="E34 E36:E39">
     <cfRule type="expression" dxfId="11" priority="13" stopIfTrue="1">
-      <formula>OR(D35="S",D35="Ma",D35="mi",D35="cl",D35="Q")</formula>
+      <formula>OR(E34="S",E34="Ma",E34="mi",E34="cl",E34="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="10" priority="14" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D36">
+  <conditionalFormatting sqref="E35">
     <cfRule type="expression" dxfId="9" priority="11" stopIfTrue="1">
-      <formula>OR(D36="S",D36="Ma",D36="mi",D36="cl",D36="Q")</formula>
+      <formula>OR(E35="S",E35="Ma",E35="mi",E35="cl",E35="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="8" priority="12" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D26">
+  <conditionalFormatting sqref="E25">
     <cfRule type="expression" dxfId="7" priority="9" stopIfTrue="1">
-      <formula>OR(D26="S",D26="Ma",D26="mi",D26="cl",D26="Q")</formula>
+      <formula>OR(E25="S",E25="Ma",E25="mi",E25="cl",E25="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="6" priority="10" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
+  <conditionalFormatting sqref="E9">
     <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
-      <formula>OR(D10="S",D10="Ma",D10="mi",D10="cl",D10="Q")</formula>
+      <formula>OR(E9="S",E9="Ma",E9="mi",E9="cl",E9="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="4" priority="6" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13">
+  <conditionalFormatting sqref="E12">
     <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>OR(D13="S",D13="Ma",D13="mi",D13="cl",D13="Q")</formula>
+      <formula>OR(E12="S",E12="Ma",E12="mi",E12="cl",E12="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="2" priority="4" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D14:D20">
+  <conditionalFormatting sqref="E13:E19">
     <cfRule type="expression" dxfId="1" priority="1" stopIfTrue="1">
-      <formula>OR(D14="S",D14="Ma",D14="mi",D14="cl",D14="Q")</formula>
+      <formula>OR(E13="S",E13="Ma",E13="mi",E13="cl",E13="Q")</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="0" priority="2" stopIfTrue="1" operator="notEqual">
       <formula>""</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D57">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E56">
       <formula1>"D,Q,E"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G6:G57 E6:E57">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H6:H56 F6:F56">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2528,21 +2575,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006DF22D4ED0D65744A5324CFBF61E7267" ma:contentTypeVersion="0" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1c7d39199afebea215da257a1a8442a7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1b05d82d297216baf5b26c55225140df">
     <xsd:element name="properties">
@@ -2656,15 +2694,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1320B1-D764-4C81-9B48-5F60482C3805}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2679,7 +2718,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ECFFD0C5-71AF-43FC-BB9C-C9954D60B2E6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2693,4 +2732,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0F20991C-9C75-4A23-AD56-83877EA734AB}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>